<commit_message>
updated with pop tree
</commit_message>
<xml_diff>
--- a/data/census_data/acs_5yr_dp_var.xlsx
+++ b/data/census_data/acs_5yr_dp_var.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\housing-dash\data\census_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CF1A6D-4E48-440A-BE7A-FC303851A781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A70BA6-46F4-4B16-B249-98B26F87D33E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27555" yWindow="1245" windowWidth="26325" windowHeight="15195" xr2:uid="{E4B61A52-3081-43B9-A6F3-4657E1DFF1A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E4B61A52-3081-43B9-A6F3-4657E1DFF1A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5838,7 +5838,7 @@
   <dimension ref="A1:K1349"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1202" sqref="D1202"/>
+      <selection activeCell="C30" sqref="A30:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5886,7 +5886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -5944,7 +5944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -6078,7 +6078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -6224,7 +6224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -6370,7 +6370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -6516,7 +6516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -6580,7 +6580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -6650,7 +6650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -6918,7 +6918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -7040,7 +7040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -7104,7 +7104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -7232,7 +7232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -7296,7 +7296,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -7430,7 +7430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -7488,7 +7488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -7552,7 +7552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -7616,7 +7616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -7744,7 +7744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -7866,7 +7866,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -7930,7 +7930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -7994,7 +7994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -8058,7 +8058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -8122,7 +8122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>73</v>
       </c>
@@ -8186,7 +8186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -8244,7 +8244,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -8308,7 +8308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>79</v>
       </c>
@@ -8378,7 +8378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>81</v>
       </c>
@@ -8442,7 +8442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>83</v>
       </c>
@@ -8506,7 +8506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>85</v>
       </c>
@@ -8570,7 +8570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -8634,7 +8634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>89</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -8756,7 +8756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -8826,7 +8826,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -8896,7 +8896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>97</v>
       </c>
@@ -8966,7 +8966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>99</v>
       </c>
@@ -9036,7 +9036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>101</v>
       </c>
@@ -9094,7 +9094,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>103</v>
       </c>
@@ -9158,7 +9158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>105</v>
       </c>
@@ -9222,7 +9222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>107</v>
       </c>
@@ -9280,7 +9280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>109</v>
       </c>
@@ -9344,7 +9344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>111</v>
       </c>
@@ -9408,7 +9408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>113</v>
       </c>
@@ -9472,7 +9472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>115</v>
       </c>
@@ -9536,7 +9536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>117</v>
       </c>
@@ -9600,7 +9600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>119</v>
       </c>
@@ -9658,7 +9658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>121</v>
       </c>
@@ -9722,7 +9722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>123</v>
       </c>
@@ -9786,7 +9786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>125</v>
       </c>
@@ -9850,7 +9850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>127</v>
       </c>
@@ -9914,7 +9914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>129</v>
       </c>
@@ -9978,7 +9978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>131</v>
       </c>
@@ -10042,7 +10042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>133</v>
       </c>
@@ -10106,7 +10106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>135</v>
       </c>
@@ -10170,7 +10170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>137</v>
       </c>
@@ -10234,7 +10234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>139</v>
       </c>
@@ -10292,7 +10292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>141</v>
       </c>
@@ -10356,7 +10356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>143</v>
       </c>
@@ -10414,7 +10414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>145</v>
       </c>
@@ -10478,7 +10478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>147</v>
       </c>
@@ -10536,7 +10536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>149</v>
       </c>
@@ -10600,7 +10600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>151</v>
       </c>
@@ -10658,7 +10658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>153</v>
       </c>
@@ -10722,7 +10722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>155</v>
       </c>
@@ -10780,7 +10780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>157</v>
       </c>
@@ -10844,7 +10844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>159</v>
       </c>
@@ -10902,7 +10902,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>161</v>
       </c>
@@ -10966,7 +10966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>163</v>
       </c>
@@ -11030,7 +11030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>165</v>
       </c>
@@ -11100,7 +11100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>167</v>
       </c>
@@ -11170,7 +11170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>169</v>
       </c>
@@ -11246,7 +11246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>171</v>
       </c>
@@ -11322,7 +11322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>173</v>
       </c>
@@ -11386,7 +11386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>175</v>
       </c>
@@ -11444,7 +11444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>177</v>
       </c>
@@ -11508,7 +11508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>179</v>
       </c>
@@ -11578,7 +11578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>181</v>
       </c>
@@ -11654,7 +11654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>183</v>
       </c>
@@ -11730,7 +11730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>185</v>
       </c>
@@ -11800,7 +11800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>187</v>
       </c>
@@ -11864,7 +11864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>189</v>
       </c>
@@ -11922,7 +11922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>191</v>
       </c>
@@ -11986,7 +11986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>193</v>
       </c>
@@ -12050,7 +12050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>195</v>
       </c>
@@ -12108,7 +12108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="194" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>197</v>
       </c>
@@ -12172,7 +12172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>199</v>
       </c>
@@ -12242,7 +12242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>201</v>
       </c>
@@ -12312,7 +12312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>203</v>
       </c>
@@ -12376,7 +12376,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>205</v>
       </c>
@@ -12446,7 +12446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>207</v>
       </c>
@@ -12516,7 +12516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>209</v>
       </c>
@@ -12574,7 +12574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>211</v>
       </c>
@@ -12638,7 +12638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>213</v>
       </c>
@@ -12702,7 +12702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>215</v>
       </c>
@@ -12766,7 +12766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>217</v>
       </c>
@@ -12830,7 +12830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>219</v>
       </c>
@@ -12894,7 +12894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>221</v>
       </c>
@@ -12958,7 +12958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>223</v>
       </c>
@@ -13016,7 +13016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>225</v>
       </c>
@@ -13080,7 +13080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>227</v>
       </c>
@@ -13144,7 +13144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>229</v>
       </c>
@@ -13214,7 +13214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>231</v>
       </c>
@@ -13278,7 +13278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>233</v>
       </c>
@@ -13348,7 +13348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>235</v>
       </c>
@@ -13412,7 +13412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>237</v>
       </c>
@@ -13482,7 +13482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>239</v>
       </c>
@@ -13546,7 +13546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="238" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>241</v>
       </c>
@@ -13616,7 +13616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>243</v>
       </c>
@@ -13680,7 +13680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>245</v>
       </c>
@@ -13750,7 +13750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>247</v>
       </c>
@@ -13808,7 +13808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>249</v>
       </c>
@@ -13872,7 +13872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>251</v>
       </c>
@@ -13936,7 +13936,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>253</v>
       </c>
@@ -14000,7 +14000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>255</v>
       </c>
@@ -14064,7 +14064,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>257</v>
       </c>
@@ -14128,7 +14128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>259</v>
       </c>
@@ -14192,7 +14192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="258" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>261</v>
       </c>
@@ -14256,7 +14256,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="260" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>263</v>
       </c>
@@ -14320,7 +14320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>265</v>
       </c>
@@ -14384,7 +14384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>267</v>
       </c>
@@ -14448,7 +14448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="266" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>269</v>
       </c>
@@ -14512,7 +14512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="268" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>271</v>
       </c>
@@ -14576,7 +14576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>273</v>
       </c>
@@ -14640,7 +14640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="272" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>275</v>
       </c>
@@ -14704,7 +14704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>277</v>
       </c>
@@ -14768,7 +14768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>279</v>
       </c>
@@ -14832,7 +14832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>281</v>
       </c>
@@ -14896,7 +14896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>283</v>
       </c>
@@ -14960,7 +14960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="282" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>285</v>
       </c>
@@ -15024,7 +15024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>287</v>
       </c>
@@ -15088,7 +15088,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="286" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>289</v>
       </c>
@@ -15152,7 +15152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>291</v>
       </c>
@@ -15216,7 +15216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>293</v>
       </c>
@@ -15280,7 +15280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>295</v>
       </c>
@@ -15344,7 +15344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="294" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>297</v>
       </c>
@@ -15408,7 +15408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="296" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>299</v>
       </c>
@@ -15472,7 +15472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="298" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>301</v>
       </c>
@@ -15536,7 +15536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="300" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>303</v>
       </c>
@@ -15594,7 +15594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="302" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>305</v>
       </c>
@@ -15658,7 +15658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="304" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>307</v>
       </c>
@@ -43568,7 +43568,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="1170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1170" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1170" t="s">
         <v>1176</v>
       </c>
@@ -43626,7 +43626,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1172" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1172" t="s">
         <v>1179</v>
       </c>
@@ -43690,7 +43690,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1174" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1174" t="s">
         <v>1181</v>
       </c>
@@ -43754,7 +43754,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1176" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1176" t="s">
         <v>1183</v>
       </c>
@@ -43818,7 +43818,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1178" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1178" t="s">
         <v>1185</v>
       </c>
@@ -43882,7 +43882,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1180" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1180" t="s">
         <v>1187</v>
       </c>
@@ -43946,7 +43946,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1182" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1182" t="s">
         <v>1189</v>
       </c>
@@ -44010,7 +44010,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1184" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1184" t="s">
         <v>1191</v>
       </c>
@@ -44074,7 +44074,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1186" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1186" t="s">
         <v>1193</v>
       </c>
@@ -44138,7 +44138,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1188" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1188" t="s">
         <v>1195</v>
       </c>
@@ -44202,7 +44202,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1190" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1190" t="s">
         <v>1197</v>
       </c>
@@ -44266,7 +44266,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1192" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1192" t="s">
         <v>1199</v>
       </c>
@@ -44330,7 +44330,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1194" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1194" t="s">
         <v>1201</v>
       </c>
@@ -44394,7 +44394,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1196" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1196" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1196" t="s">
         <v>1203</v>
       </c>
@@ -44458,7 +44458,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1198" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1198" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1198" t="s">
         <v>1205</v>
       </c>
@@ -44522,7 +44522,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1200" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1200" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1200" t="s">
         <v>1207</v>
       </c>
@@ -44586,7 +44586,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1202" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1202" t="s">
         <v>1209</v>
       </c>
@@ -44650,7 +44650,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1204" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1204" t="s">
         <v>1211</v>
       </c>
@@ -44714,7 +44714,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1206" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1206" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1206" t="s">
         <v>1213</v>
       </c>
@@ -44778,7 +44778,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1208" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1208" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1208" t="s">
         <v>1215</v>
       </c>
@@ -44842,7 +44842,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1210" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1210" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1210" t="s">
         <v>1217</v>
       </c>
@@ -44906,7 +44906,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1212" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1212" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1212" t="s">
         <v>1219</v>
       </c>
@@ -44970,7 +44970,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1214" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1214" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1214" t="s">
         <v>1221</v>
       </c>
@@ -45034,7 +45034,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1216" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1216" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1216" t="s">
         <v>1223</v>
       </c>
@@ -45098,7 +45098,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1218" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1218" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1218" t="s">
         <v>1225</v>
       </c>
@@ -45162,7 +45162,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1220" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1220" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1220" t="s">
         <v>1227</v>
       </c>
@@ -45232,7 +45232,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1222" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1222" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1222" t="s">
         <v>1229</v>
       </c>
@@ -45302,7 +45302,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1224" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1224" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1224" t="s">
         <v>1231</v>
       </c>
@@ -45372,7 +45372,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1226" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1226" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1226" t="s">
         <v>1233</v>
       </c>
@@ -45436,7 +45436,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1228" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1228" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1228" t="s">
         <v>1235</v>
       </c>
@@ -45506,7 +45506,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1230" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1230" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1230" t="s">
         <v>1237</v>
       </c>
@@ -45576,7 +45576,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1232" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1232" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1232" t="s">
         <v>1239</v>
       </c>
@@ -45646,7 +45646,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1234" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1234" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1234" t="s">
         <v>1241</v>
       </c>
@@ -45704,7 +45704,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1236" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1236" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1236" t="s">
         <v>1243</v>
       </c>
@@ -45768,7 +45768,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1238" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1238" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1238" t="s">
         <v>1245</v>
       </c>
@@ -45832,7 +45832,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1240" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1240" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1240" t="s">
         <v>1247</v>
       </c>
@@ -45896,7 +45896,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1242" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1242" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1242" t="s">
         <v>1249</v>
       </c>
@@ -45966,7 +45966,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1244" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1244" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1244" t="s">
         <v>1251</v>
       </c>
@@ -46036,7 +46036,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1246" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1246" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1246" t="s">
         <v>1253</v>
       </c>
@@ -46106,7 +46106,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1248" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1248" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1248" t="s">
         <v>1255</v>
       </c>
@@ -46182,7 +46182,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1250" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1250" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1250" t="s">
         <v>1257</v>
       </c>
@@ -46258,7 +46258,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1252" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1252" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1252" t="s">
         <v>1259</v>
       </c>
@@ -46334,7 +46334,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1254" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1254" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1254" t="s">
         <v>1261</v>
       </c>
@@ -46410,7 +46410,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1256" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1256" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1256" t="s">
         <v>1263</v>
       </c>
@@ -46480,7 +46480,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1258" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1258" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1258" t="s">
         <v>1265</v>
       </c>
@@ -46556,7 +46556,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1260" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1260" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1260" t="s">
         <v>1267</v>
       </c>
@@ -46632,7 +46632,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1262" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1262" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1262" t="s">
         <v>1269</v>
       </c>
@@ -46708,7 +46708,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1264" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1264" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1264" t="s">
         <v>1271</v>
       </c>
@@ -46784,7 +46784,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1266" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1266" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1266" t="s">
         <v>1273</v>
       </c>
@@ -46860,7 +46860,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1268" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1268" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1268" t="s">
         <v>1275</v>
       </c>
@@ -46936,7 +46936,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1270" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1270" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1270" t="s">
         <v>1277</v>
       </c>
@@ -47012,7 +47012,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1272" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1272" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1272" t="s">
         <v>1279</v>
       </c>
@@ -47082,7 +47082,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1274" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1274" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1274" t="s">
         <v>1281</v>
       </c>
@@ -47158,7 +47158,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1276" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1276" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1276" t="s">
         <v>1283</v>
       </c>
@@ -47234,7 +47234,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1278" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1278" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1278" t="s">
         <v>1285</v>
       </c>
@@ -47310,7 +47310,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1280" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1280" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1280" t="s">
         <v>1287</v>
       </c>
@@ -47386,7 +47386,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1282" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1282" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1282" t="s">
         <v>1289</v>
       </c>
@@ -47456,7 +47456,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1284" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1284" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1284" t="s">
         <v>1291</v>
       </c>
@@ -47520,7 +47520,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1286" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1286" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1286" t="s">
         <v>1293</v>
       </c>
@@ -47590,7 +47590,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1288" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1288" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1288" t="s">
         <v>1295</v>
       </c>
@@ -47660,7 +47660,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1290" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1290" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1290" t="s">
         <v>1297</v>
       </c>
@@ -47730,7 +47730,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1292" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1292" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1292" t="s">
         <v>1299</v>
       </c>
@@ -47800,7 +47800,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1294" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1294" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1294" t="s">
         <v>1301</v>
       </c>
@@ -47858,7 +47858,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1296" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1296" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1296" t="s">
         <v>1303</v>
       </c>
@@ -47922,7 +47922,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1298" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1298" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1298" t="s">
         <v>1305</v>
       </c>
@@ -47986,7 +47986,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1300" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1300" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1300" t="s">
         <v>1307</v>
       </c>
@@ -48050,7 +48050,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1302" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1302" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1302" t="s">
         <v>1309</v>
       </c>
@@ -48114,7 +48114,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1304" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1304" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1304" t="s">
         <v>1311</v>
       </c>
@@ -48178,7 +48178,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1306" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1306" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1306" t="s">
         <v>1313</v>
       </c>
@@ -48242,7 +48242,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1308" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1308" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1308" t="s">
         <v>1315</v>
       </c>
@@ -48300,7 +48300,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1310" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1310" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1310" t="s">
         <v>1317</v>
       </c>
@@ -48364,7 +48364,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1312" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1312" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1312" t="s">
         <v>1319</v>
       </c>
@@ -48434,7 +48434,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1314" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1314" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1314" t="s">
         <v>1321</v>
       </c>
@@ -48504,7 +48504,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1316" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1316" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1316" t="s">
         <v>1323</v>
       </c>
@@ -48574,7 +48574,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1318" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1318" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1318" t="s">
         <v>1325</v>
       </c>
@@ -48644,7 +48644,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1320" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1320" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1320" t="s">
         <v>1327</v>
       </c>
@@ -48708,7 +48708,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1322" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1322" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1322" t="s">
         <v>1329</v>
       </c>
@@ -48778,7 +48778,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1324" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1324" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1324" t="s">
         <v>1331</v>
       </c>
@@ -48848,7 +48848,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1326" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1326" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1326" t="s">
         <v>1333</v>
       </c>
@@ -48918,7 +48918,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1328" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1328" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1328" t="s">
         <v>1335</v>
       </c>
@@ -48988,7 +48988,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1330" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1330" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1330" t="s">
         <v>1337</v>
       </c>
@@ -49058,7 +49058,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1332" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1332" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1332" t="s">
         <v>1339</v>
       </c>
@@ -49128,7 +49128,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1334" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1334" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1334" t="s">
         <v>1341</v>
       </c>
@@ -49198,7 +49198,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1336" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1336" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1336" t="s">
         <v>1343</v>
       </c>
@@ -49274,7 +49274,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1338" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1338" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1338" t="s">
         <v>1345</v>
       </c>
@@ -49350,7 +49350,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1340" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1340" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1340" t="s">
         <v>1347</v>
       </c>
@@ -49402,7 +49402,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1342" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1342" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1342" t="s">
         <v>1349</v>
       </c>
@@ -49460,7 +49460,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1344" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1344" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1344" t="s">
         <v>1351</v>
       </c>
@@ -49524,7 +49524,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="1346" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1346" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1346" t="s">
         <v>1353</v>
       </c>
@@ -49634,7 +49634,7 @@
     </filterColumn>
     <filterColumn colId="10">
       <filters>
-        <filter val="DP05"/>
+        <filter val="DP02"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>